<commit_message>
Avance de documentación de proyecto
</commit_message>
<xml_diff>
--- a/Documentación del proyecto/Planilla de requerimientos.xlsx
+++ b/Documentación del proyecto/Planilla de requerimientos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manu_\Desktop\Proyecto de arquitectura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manu_\Desktop\Proyecto de arquitectura\Documentación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E707FB-5310-4C40-9DFC-E7BAD5A87EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A2E062-3B90-4C2B-AF4D-00553C6D4E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -812,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>